<commit_message>
added functions for code readability and mudalarity. changed models to partitioned models (10 - fold) for better evaluation. some more changes in plots, correlations and more
</commit_message>
<xml_diff>
--- a/known_data_set.xlsx
+++ b/known_data_set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirelitzur/Documents/MATLAB/M&amp;T/challenge_2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E18C428-56B2-4A4F-98D9-37876FDFAA10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B95309-6A06-324E-BF0C-0BE5D2F56BB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BS540"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AJ10" sqref="AJ10"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="95" workbookViewId="0">
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -574,7 +574,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>1</v>
@@ -583,7 +583,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>1</v>
@@ -592,7 +592,7 @@
         <v>1</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>1</v>
@@ -601,7 +601,7 @@
         <v>1</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>1</v>
@@ -610,7 +610,7 @@
         <v>1</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q1" s="3" t="s">
         <v>1</v>
@@ -619,7 +619,7 @@
         <v>1</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T1" s="3" t="s">
         <v>1</v>
@@ -628,7 +628,7 @@
         <v>1</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W1" s="3" t="s">
         <v>1</v>
@@ -637,7 +637,7 @@
         <v>1</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z1" s="3" t="s">
         <v>1</v>

</xml_diff>